<commit_message>
Relatorio pre pronto. SERA ?
</commit_message>
<xml_diff>
--- a/EXP_2/Tabelas_EXP_2.xlsx
+++ b/EXP_2/Tabelas_EXP_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Filho\Documents\FISICA_1\EXP_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D56792E-6699-44DE-9A07-27F951845756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF8B2ED-2620-4A3E-8937-B3529C364692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31890" yWindow="3885" windowWidth="21600" windowHeight="11505" xr2:uid="{FCFF52A2-2253-4303-A898-002B8F5738EB}"/>
+    <workbookView xWindow="-3070" yWindow="-10910" windowWidth="19420" windowHeight="10560" xr2:uid="{FCFF52A2-2253-4303-A898-002B8F5738EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
   <si>
     <t>Medidas</t>
   </si>
@@ -87,13 +109,53 @@
   <si>
     <t>0.480</t>
   </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Desvio</t>
+  </si>
+  <si>
+    <t>Desvio Tempo</t>
+  </si>
+  <si>
+    <t>Desvio Médio</t>
+  </si>
+  <si>
+    <t>&lt;t1&gt;-&lt;t2&gt;</t>
+  </si>
+  <si>
+    <t>Cálculos finais</t>
+  </si>
+  <si>
+    <t>&lt;t1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;t2&gt;</t>
+  </si>
+  <si>
+    <t>3t1</t>
+  </si>
+  <si>
+    <t>2t1</t>
+  </si>
+  <si>
+    <t>Dados Incompatíveis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -126,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +213,32 @@
         <bgColor theme="1" tint="0.44999542222357858"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor theme="1" tint="0.44999542222357858"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor theme="1" tint="0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -209,12 +295,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,24 +401,131 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -292,52 +546,13 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -361,13 +576,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -439,7 +657,43 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -490,31 +744,178 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>116173</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>192373</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>187325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5919F0A5-54AD-9783-CFB7-07BCBE66FCD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14429820" y="5827059"/>
+          <a:ext cx="76200" cy="187325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>105527</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>181727</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>187325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C81E81-1FC8-72AB-0933-CFB2C3C6DD9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14419174" y="6021294"/>
+          <a:ext cx="76200" cy="187325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C5F1F445-0E83-4789-9939-E36214064FB3}" name="Tabela14" displayName="Tabela14" ref="A4:F24" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A4:F24" xr:uid="{C5F1F445-0E83-4789-9939-E36214064FB3}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{30ACD64F-E1BE-4B3E-880C-43BB771C3BC5}" name="Medidas" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{DC9D8557-BB50-4596-BD37-DC510E513C9A}" name="Tempo (s)" dataDxfId="3" dataCellStyle="Vírgula"/>
-    <tableColumn id="4" xr3:uid="{8FFB3F4C-2188-421A-8F2C-84A2E16CA841}" name="Medidas2" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CDB84458-0210-4E31-A57C-9BD278BCEF13}" name="Tempo (s)3" dataDxfId="2" dataCellStyle="Vírgula"/>
-    <tableColumn id="7" xr3:uid="{D6889D63-9585-4B66-8797-F48BBFBA0CD7}" name="Medidas5" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{E5DE78CF-1415-46B3-97D4-7A337B7503B8}" name="Tempo (s)6" dataDxfId="10" dataCellStyle="Vírgula"/>
+    <tableColumn id="2" xr3:uid="{DC9D8557-BB50-4596-BD37-DC510E513C9A}" name="Tempo (s)" dataDxfId="12" dataCellStyle="Vírgula"/>
+    <tableColumn id="4" xr3:uid="{8FFB3F4C-2188-421A-8F2C-84A2E16CA841}" name="Medidas2" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{CDB84458-0210-4E31-A57C-9BD278BCEF13}" name="Tempo (s)3" dataDxfId="10" dataCellStyle="Vírgula"/>
+    <tableColumn id="7" xr3:uid="{D6889D63-9585-4B66-8797-F48BBFBA0CD7}" name="Medidas5" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{E5DE78CF-1415-46B3-97D4-7A337B7503B8}" name="Tempo (s)6" dataDxfId="8" dataCellStyle="Vírgula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{47F1162E-E622-49CD-8891-91C814C1E92A}" name="Tabela1417" displayName="Tabela1417" ref="A29:F49" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{47F1162E-E622-49CD-8891-91C814C1E92A}" name="Tabela1417" displayName="Tabela1417" ref="A29:F49" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A29:F49" xr:uid="{47F1162E-E622-49CD-8891-91C814C1E92A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2EBD7A43-2F99-42B9-9209-8AF2145A3C6B}" name="Medidas" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{0097D0F3-CBB0-4E04-90DE-8011500277AA}" name="Tempo (s)" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{D7691C81-C949-47EA-B65C-B2BEB9AE25C3}" name="Medidas2" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{A76759C2-B580-4F67-8F5B-D3DBE4AE2806}" name="Tempo (s)3" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{C0820B21-5F7A-4B71-85AA-658670891EFA}" name="Medidas5" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{BEE86FAB-72A5-4DD4-AEAF-E3DC557CF94D}" name="Tempo (s)6" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{2EBD7A43-2F99-42B9-9209-8AF2145A3C6B}" name="Medidas" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0097D0F3-CBB0-4E04-90DE-8011500277AA}" name="Tempo (s)" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{D7691C81-C949-47EA-B65C-B2BEB9AE25C3}" name="Medidas2" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A76759C2-B580-4F67-8F5B-D3DBE4AE2806}" name="Tempo (s)3" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{C0820B21-5F7A-4B71-85AA-658670891EFA}" name="Medidas5" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{BEE86FAB-72A5-4DD4-AEAF-E3DC557CF94D}" name="Tempo (s)6" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -817,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC65827-CCCF-4375-835F-E03FB3F4C1AD}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="E21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32:V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,48 +1234,61 @@
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="L1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -893,19 +1307,34 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="18" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -924,11 +1353,11 @@
       <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22" t="s">
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="3"/>
@@ -936,7 +1365,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -955,19 +1384,37 @@
       <c r="F5" s="11">
         <v>0.5</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="23" t="s">
+      <c r="H5" s="22"/>
+      <c r="I5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" s="25">
+        <v>1</v>
+      </c>
+      <c r="M5" s="37">
+        <f xml:space="preserve"> SUM(B5-$H$24)</f>
+        <v>2.3833333333333151E-2</v>
+      </c>
+      <c r="N5" s="25">
+        <v>21</v>
+      </c>
+      <c r="O5" s="37">
+        <f xml:space="preserve"> SUM(D5-$H$24)</f>
+        <v>7.3833333333333195E-2</v>
+      </c>
+      <c r="P5" s="25">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="39">
+        <f xml:space="preserve"> SUM(F5-$H$24)</f>
+        <v>2.3833333333333151E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -986,21 +1433,39 @@
       <c r="F6" s="11">
         <v>0.5</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="29" t="s">
         <v>13</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="26">
+        <v>2</v>
+      </c>
+      <c r="M6" s="38">
+        <f t="shared" ref="M6:M23" si="0" xml:space="preserve"> SUM(B6-$H$24)</f>
+        <v>-0.14616666666666683</v>
+      </c>
+      <c r="N6" s="26">
+        <v>22</v>
+      </c>
+      <c r="O6" s="38">
+        <f t="shared" ref="O6:O24" si="1" xml:space="preserve"> SUM(D6-$H$24)</f>
+        <v>3.383333333333316E-2</v>
+      </c>
+      <c r="P6" s="26">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="40">
+        <f t="shared" ref="Q6:Q24" si="2" xml:space="preserve"> SUM(F6-$H$24)</f>
+        <v>2.3833333333333151E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -1023,11 +1488,29 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="25">
+        <v>3</v>
+      </c>
+      <c r="M7" s="37">
+        <f t="shared" si="0"/>
+        <v>-6.6166666666666873E-2</v>
+      </c>
+      <c r="N7" s="25">
+        <v>23</v>
+      </c>
+      <c r="O7" s="37">
+        <f t="shared" si="1"/>
+        <v>-0.11616666666666686</v>
+      </c>
+      <c r="P7" s="25">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="39">
+        <f t="shared" si="2"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -1046,17 +1529,35 @@
       <c r="F8" s="11">
         <v>0.48</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="26">
+        <v>4</v>
+      </c>
+      <c r="M8" s="38">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333151E-2</v>
+      </c>
+      <c r="N8" s="26">
+        <v>24</v>
+      </c>
+      <c r="O8" s="38">
+        <f t="shared" si="1"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+      <c r="P8" s="26">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="40">
+        <f t="shared" si="2"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -1075,15 +1576,33 @@
       <c r="F9" s="11">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="25">
+        <v>5</v>
+      </c>
+      <c r="M9" s="37">
+        <f t="shared" si="0"/>
+        <v>-7.6166666666666827E-2</v>
+      </c>
+      <c r="N9" s="25">
+        <v>25</v>
+      </c>
+      <c r="O9" s="37">
+        <f t="shared" si="1"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+      <c r="P9" s="25">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="39">
+        <f t="shared" si="2"/>
+        <v>9.3833333333333102E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -1102,19 +1621,39 @@
       <c r="F10" s="11">
         <v>0.42</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="22"/>
+      <c r="I10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="26">
+        <v>6</v>
+      </c>
+      <c r="M10" s="38">
+        <f t="shared" si="0"/>
+        <v>3.383333333333316E-2</v>
+      </c>
+      <c r="N10" s="26">
+        <v>26</v>
+      </c>
+      <c r="O10" s="38">
+        <f t="shared" si="1"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+      <c r="P10" s="26">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="40">
+        <f t="shared" si="2"/>
+        <v>-5.6166666666666865E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -1133,19 +1672,37 @@
       <c r="F11" s="11">
         <v>0.45</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="23" t="s">
+      <c r="H11" s="22"/>
+      <c r="I11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="25">
+        <v>7</v>
+      </c>
+      <c r="M11" s="37">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333151E-2</v>
+      </c>
+      <c r="N11" s="25">
+        <v>27</v>
+      </c>
+      <c r="O11" s="37">
+        <f t="shared" si="1"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+      <c r="P11" s="25">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="39">
+        <f t="shared" si="2"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -1164,21 +1721,39 @@
       <c r="F12" s="11">
         <v>0.46</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="29" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L12" s="26">
+        <v>8</v>
+      </c>
+      <c r="M12" s="38">
+        <f t="shared" si="0"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+      <c r="N12" s="26">
+        <v>28</v>
+      </c>
+      <c r="O12" s="38">
+        <f t="shared" si="1"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+      <c r="P12" s="26">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="40">
+        <f t="shared" si="2"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -1201,11 +1776,29 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L13" s="25">
+        <v>9</v>
+      </c>
+      <c r="M13" s="37">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333151E-2</v>
+      </c>
+      <c r="N13" s="25">
+        <v>29</v>
+      </c>
+      <c r="O13" s="37">
+        <f t="shared" si="1"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+      <c r="P13" s="25">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="39">
+        <f t="shared" si="2"/>
+        <v>0.13383333333333314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -1228,11 +1821,29 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="26">
+        <v>10</v>
+      </c>
+      <c r="M14" s="38">
+        <f t="shared" si="0"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+      <c r="N14" s="26">
+        <v>30</v>
+      </c>
+      <c r="O14" s="38">
+        <f t="shared" si="1"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+      <c r="P14" s="26">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="40">
+        <f t="shared" si="2"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -1255,11 +1866,29 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="25">
+        <v>11</v>
+      </c>
+      <c r="M15" s="37">
+        <f t="shared" si="0"/>
+        <v>-4.6166666666666856E-2</v>
+      </c>
+      <c r="N15" s="25">
+        <v>31</v>
+      </c>
+      <c r="O15" s="37">
+        <f t="shared" si="1"/>
+        <v>-4.6166666666666856E-2</v>
+      </c>
+      <c r="P15" s="25">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="39">
+        <f t="shared" si="2"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -1278,15 +1907,32 @@
       <c r="F16" s="11">
         <v>0.48</v>
       </c>
-      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" s="26">
+        <v>12</v>
+      </c>
+      <c r="M16" s="38">
+        <f t="shared" si="0"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+      <c r="N16" s="26">
+        <v>32</v>
+      </c>
+      <c r="O16" s="38">
+        <f t="shared" si="1"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+      <c r="P16" s="26">
+        <v>52</v>
+      </c>
+      <c r="Q16" s="40">
+        <f t="shared" si="2"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -1305,15 +1951,32 @@
       <c r="F17" s="11">
         <v>0.48</v>
       </c>
-      <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="25">
+        <v>13</v>
+      </c>
+      <c r="M17" s="37">
+        <f t="shared" si="0"/>
+        <v>-8.6166666666666836E-2</v>
+      </c>
+      <c r="N17" s="25">
+        <v>33</v>
+      </c>
+      <c r="O17" s="37">
+        <f t="shared" si="1"/>
+        <v>0.10383333333333311</v>
+      </c>
+      <c r="P17" s="25">
+        <v>53</v>
+      </c>
+      <c r="Q17" s="39">
+        <f t="shared" si="2"/>
+        <v>3.8333333333331332E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -1336,11 +1999,29 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="26">
+        <v>14</v>
+      </c>
+      <c r="M18" s="38">
+        <f t="shared" si="0"/>
+        <v>-4.6166666666666856E-2</v>
+      </c>
+      <c r="N18" s="26">
+        <v>34</v>
+      </c>
+      <c r="O18" s="38">
+        <f t="shared" si="1"/>
+        <v>3.383333333333316E-2</v>
+      </c>
+      <c r="P18" s="26">
+        <v>54</v>
+      </c>
+      <c r="Q18" s="40">
+        <f t="shared" si="2"/>
+        <v>7.3833333333333195E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -1363,11 +2044,29 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="25">
+        <v>15</v>
+      </c>
+      <c r="M19" s="37">
+        <f t="shared" si="0"/>
+        <v>5.3833333333333178E-2</v>
+      </c>
+      <c r="N19" s="25">
+        <v>35</v>
+      </c>
+      <c r="O19" s="37">
+        <f t="shared" si="1"/>
+        <v>5.3833333333333178E-2</v>
+      </c>
+      <c r="P19" s="25">
+        <v>55</v>
+      </c>
+      <c r="Q19" s="39">
+        <f t="shared" si="2"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>16</v>
       </c>
@@ -1390,11 +2089,29 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="26">
+        <v>16</v>
+      </c>
+      <c r="M20" s="38">
+        <f t="shared" si="0"/>
+        <v>7.3833333333333195E-2</v>
+      </c>
+      <c r="N20" s="26">
+        <v>36</v>
+      </c>
+      <c r="O20" s="38">
+        <f t="shared" si="1"/>
+        <v>9.3833333333333102E-2</v>
+      </c>
+      <c r="P20" s="26">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="40">
+        <f t="shared" si="2"/>
+        <v>3.383333333333316E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>17</v>
       </c>
@@ -1417,11 +2134,29 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="25">
+        <v>17</v>
+      </c>
+      <c r="M21" s="37">
+        <f t="shared" si="0"/>
+        <v>-4.6166666666666856E-2</v>
+      </c>
+      <c r="N21" s="25">
+        <v>37</v>
+      </c>
+      <c r="O21" s="37">
+        <f t="shared" si="1"/>
+        <v>3.383333333333316E-2</v>
+      </c>
+      <c r="P21" s="25">
+        <v>57</v>
+      </c>
+      <c r="Q21" s="39">
+        <f t="shared" si="2"/>
+        <v>-6.6166666666666873E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -1444,11 +2179,29 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="26">
+        <v>18</v>
+      </c>
+      <c r="M22" s="38">
+        <f t="shared" si="0"/>
+        <v>-4.6166666666666856E-2</v>
+      </c>
+      <c r="N22" s="26">
+        <v>38</v>
+      </c>
+      <c r="O22" s="38">
+        <f t="shared" si="1"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+      <c r="P22" s="26">
+        <v>58</v>
+      </c>
+      <c r="Q22" s="40">
+        <f t="shared" si="2"/>
+        <v>-6.1666666666668757E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>19</v>
       </c>
@@ -1467,15 +2220,37 @@
       <c r="F23" s="11">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="H23" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>17</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="25">
+        <v>19</v>
+      </c>
+      <c r="M23" s="37">
+        <f t="shared" si="0"/>
+        <v>-0.12616666666666687</v>
+      </c>
+      <c r="N23" s="25">
+        <v>39</v>
+      </c>
+      <c r="O23" s="37">
+        <f t="shared" si="1"/>
+        <v>-2.6166666666666838E-2</v>
+      </c>
+      <c r="P23" s="25">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="39">
+        <f t="shared" si="2"/>
+        <v>7.3833333333333195E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>20</v>
       </c>
@@ -1494,43 +2269,99 @@
       <c r="F24" s="14">
         <v>0.46</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="23">
+        <f>SUM(B5:B24,D5:D24,F5:F24)/60</f>
+        <v>0.47616666666666685</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="26">
+        <v>20</v>
+      </c>
+      <c r="M24" s="38">
+        <f xml:space="preserve"> SUM(B24-$H$24)</f>
+        <v>0.10383333333333311</v>
+      </c>
+      <c r="N24" s="26">
+        <v>40</v>
+      </c>
+      <c r="O24" s="38">
+        <f t="shared" si="1"/>
+        <v>3.383333333333316E-2</v>
+      </c>
+      <c r="P24" s="26">
+        <v>60</v>
+      </c>
+      <c r="Q24" s="41">
+        <f t="shared" si="2"/>
+        <v>-1.6166666666666829E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E25"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="48">
+        <f>2*O25</f>
+        <v>5.3566666666666714E-2</v>
+      </c>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="L25" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="31"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="42" cm="1">
+        <f t="array" ref="O25">SUM(ABS(M5:M24+O5:O24+Q5:Q24))/60</f>
+        <v>2.6783333333333357E-2</v>
+      </c>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="44"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="H26" s="47">
+        <f>ABS(H24-H49)</f>
+        <v>0.10451666666666692</v>
+      </c>
+      <c r="J26" s="49">
+        <f>3*O25</f>
+        <v>8.0350000000000074E-2</v>
+      </c>
+      <c r="L26" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="L27" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
@@ -1549,8 +2380,26 @@
       <c r="F28" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
@@ -1569,8 +2418,14 @@
       <c r="F29" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>1</v>
       </c>
@@ -1589,8 +2444,29 @@
       <c r="F30" s="15">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L30" s="25">
+        <v>1</v>
+      </c>
+      <c r="M30" s="36">
+        <f xml:space="preserve"> SUM(B30-$H$49)</f>
+        <v>-6.6499999999999337E-3</v>
+      </c>
+      <c r="N30" s="25">
+        <v>21</v>
+      </c>
+      <c r="O30" s="36">
+        <f xml:space="preserve"> SUM(D30-$H$49)</f>
+        <v>1.3500000000000734E-3</v>
+      </c>
+      <c r="P30" s="25">
+        <v>41</v>
+      </c>
+      <c r="Q30" s="36">
+        <f xml:space="preserve"> SUM(F30-$H$49)</f>
+        <v>1.3500000000000734E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>2</v>
       </c>
@@ -1600,7 +2476,7 @@
       <c r="C31" s="10">
         <v>22</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="46">
         <v>0.37</v>
       </c>
       <c r="E31" s="10">
@@ -1609,8 +2485,29 @@
       <c r="F31" s="15">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="50">
+        <v>2</v>
+      </c>
+      <c r="M31" s="51">
+        <f t="shared" ref="M31:M49" si="3" xml:space="preserve"> SUM(B31-$H$49)</f>
+        <v>-8.6499999999999355E-3</v>
+      </c>
+      <c r="N31" s="50">
+        <v>22</v>
+      </c>
+      <c r="O31" s="51">
+        <f t="shared" ref="O31:O49" si="4" xml:space="preserve"> SUM(D31-$H$49)</f>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="P31" s="50">
+        <v>42</v>
+      </c>
+      <c r="Q31" s="51">
+        <f t="shared" ref="Q31:Q49" si="5" xml:space="preserve"> SUM(F31-$H$49)</f>
+        <v>1.3500000000000734E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>3</v>
       </c>
@@ -1629,8 +2526,36 @@
       <c r="F32" s="15">
         <v>0.36899999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J32" s="3"/>
+      <c r="L32" s="25">
+        <v>3</v>
+      </c>
+      <c r="M32" s="36">
+        <f t="shared" si="3"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+      <c r="N32" s="25">
+        <v>23</v>
+      </c>
+      <c r="O32" s="36">
+        <f t="shared" si="4"/>
+        <v>2.3500000000000743E-3</v>
+      </c>
+      <c r="P32" s="25">
+        <v>43</v>
+      </c>
+      <c r="Q32" s="36">
+        <f t="shared" si="5"/>
+        <v>-2.6499999999999302E-3</v>
+      </c>
+      <c r="S32" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="T32" s="33"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>4</v>
       </c>
@@ -1649,8 +2574,42 @@
       <c r="F33" s="15">
         <v>0.36899999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J33" s="3"/>
+      <c r="L33" s="50">
+        <v>4</v>
+      </c>
+      <c r="M33" s="51">
+        <f t="shared" si="3"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="N33" s="50">
+        <v>24</v>
+      </c>
+      <c r="O33" s="51">
+        <f t="shared" si="4"/>
+        <v>1.3500000000000734E-3</v>
+      </c>
+      <c r="P33" s="50">
+        <v>44</v>
+      </c>
+      <c r="Q33" s="51">
+        <f t="shared" si="5"/>
+        <v>-2.6499999999999302E-3</v>
+      </c>
+      <c r="S33" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="T33" s="53">
+        <v>0.48</v>
+      </c>
+      <c r="U33" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="V33" s="58">
+        <v>5.3600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>5</v>
       </c>
@@ -1669,8 +2628,41 @@
       <c r="F34" s="15">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L34" s="25">
+        <v>5</v>
+      </c>
+      <c r="M34" s="36">
+        <f t="shared" si="3"/>
+        <v>-2.6499999999999302E-3</v>
+      </c>
+      <c r="N34" s="25">
+        <v>25</v>
+      </c>
+      <c r="O34" s="36">
+        <f t="shared" si="4"/>
+        <v>4.350000000000076E-3</v>
+      </c>
+      <c r="P34" s="25">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="36">
+        <f t="shared" si="5"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="S34" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="T34" s="56">
+        <v>0.372</v>
+      </c>
+      <c r="U34" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="V34" s="60">
+        <v>8.0399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>6</v>
       </c>
@@ -1689,8 +2681,40 @@
       <c r="F35" s="15">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L35" s="50">
+        <v>6</v>
+      </c>
+      <c r="M35" s="51">
+        <f t="shared" si="3"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="N35" s="50">
+        <v>26</v>
+      </c>
+      <c r="O35" s="51">
+        <f t="shared" si="4"/>
+        <v>1.3500000000000734E-3</v>
+      </c>
+      <c r="P35" s="50">
+        <v>46</v>
+      </c>
+      <c r="Q35" s="51">
+        <f t="shared" si="5"/>
+        <v>3.3500000000000751E-3</v>
+      </c>
+      <c r="S35" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="T35" s="54">
+        <f>T33-T34</f>
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="U35" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="V35" s="62"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>7</v>
       </c>
@@ -1709,8 +2733,29 @@
       <c r="F36" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L36" s="25">
+        <v>7</v>
+      </c>
+      <c r="M36" s="36">
+        <f t="shared" si="3"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="N36" s="25">
+        <v>27</v>
+      </c>
+      <c r="O36" s="36">
+        <f t="shared" si="4"/>
+        <v>1.3500000000000734E-3</v>
+      </c>
+      <c r="P36" s="25">
+        <v>47</v>
+      </c>
+      <c r="Q36" s="36">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>8</v>
       </c>
@@ -1729,8 +2774,29 @@
       <c r="F37" s="15">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L37" s="50">
+        <v>8</v>
+      </c>
+      <c r="M37" s="51">
+        <f t="shared" si="3"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="N37" s="50">
+        <v>28</v>
+      </c>
+      <c r="O37" s="51">
+        <f t="shared" si="4"/>
+        <v>3.3500000000000751E-3</v>
+      </c>
+      <c r="P37" s="50">
+        <v>48</v>
+      </c>
+      <c r="Q37" s="51">
+        <f t="shared" si="5"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>9</v>
       </c>
@@ -1749,8 +2815,29 @@
       <c r="F38" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L38" s="25">
+        <v>9</v>
+      </c>
+      <c r="M38" s="36">
+        <f t="shared" si="3"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+      <c r="N38" s="25">
+        <v>29</v>
+      </c>
+      <c r="O38" s="36">
+        <f t="shared" si="4"/>
+        <v>2.3500000000000743E-3</v>
+      </c>
+      <c r="P38" s="25">
+        <v>49</v>
+      </c>
+      <c r="Q38" s="36">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>10</v>
       </c>
@@ -1769,8 +2856,29 @@
       <c r="F39" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L39" s="50">
+        <v>10</v>
+      </c>
+      <c r="M39" s="51">
+        <f t="shared" si="3"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+      <c r="N39" s="50">
+        <v>30</v>
+      </c>
+      <c r="O39" s="51">
+        <f t="shared" si="4"/>
+        <v>4.350000000000076E-3</v>
+      </c>
+      <c r="P39" s="50">
+        <v>50</v>
+      </c>
+      <c r="Q39" s="51">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>11</v>
       </c>
@@ -1789,8 +2897,29 @@
       <c r="F40" s="15">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L40" s="25">
+        <v>11</v>
+      </c>
+      <c r="M40" s="36">
+        <f t="shared" si="3"/>
+        <v>2.3500000000000743E-3</v>
+      </c>
+      <c r="N40" s="25">
+        <v>31</v>
+      </c>
+      <c r="O40" s="36">
+        <f t="shared" si="4"/>
+        <v>2.3500000000000743E-3</v>
+      </c>
+      <c r="P40" s="25">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="36">
+        <f t="shared" si="5"/>
+        <v>1.3500000000000734E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>12</v>
       </c>
@@ -1809,8 +2938,29 @@
       <c r="F41" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L41" s="50">
+        <v>12</v>
+      </c>
+      <c r="M41" s="51">
+        <f t="shared" si="3"/>
+        <v>-2.6499999999999302E-3</v>
+      </c>
+      <c r="N41" s="50">
+        <v>32</v>
+      </c>
+      <c r="O41" s="51">
+        <f t="shared" si="4"/>
+        <v>5.3500000000000769E-3</v>
+      </c>
+      <c r="P41" s="50">
+        <v>52</v>
+      </c>
+      <c r="Q41" s="51">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>13</v>
       </c>
@@ -1829,8 +2979,29 @@
       <c r="F42" s="15">
         <v>0.372</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L42" s="25">
+        <v>13</v>
+      </c>
+      <c r="M42" s="36">
+        <f t="shared" si="3"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+      <c r="N42" s="25">
+        <v>33</v>
+      </c>
+      <c r="O42" s="36">
+        <f t="shared" si="4"/>
+        <v>5.3500000000000769E-3</v>
+      </c>
+      <c r="P42" s="25">
+        <v>53</v>
+      </c>
+      <c r="Q42" s="36">
+        <f t="shared" si="5"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>14</v>
       </c>
@@ -1849,8 +3020,29 @@
       <c r="F43" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L43" s="50">
+        <v>14</v>
+      </c>
+      <c r="M43" s="51">
+        <f t="shared" si="3"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="N43" s="50">
+        <v>34</v>
+      </c>
+      <c r="O43" s="51">
+        <f t="shared" si="4"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="P43" s="50">
+        <v>54</v>
+      </c>
+      <c r="Q43" s="51">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>15</v>
       </c>
@@ -1869,8 +3061,29 @@
       <c r="F44" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L44" s="25">
+        <v>15</v>
+      </c>
+      <c r="M44" s="36">
+        <f t="shared" si="3"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="N44" s="25">
+        <v>35</v>
+      </c>
+      <c r="O44" s="36">
+        <f t="shared" si="4"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="P44" s="25">
+        <v>55</v>
+      </c>
+      <c r="Q44" s="36">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>16</v>
       </c>
@@ -1889,8 +3102,29 @@
       <c r="F45" s="15">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L45" s="50">
+        <v>16</v>
+      </c>
+      <c r="M45" s="51">
+        <f t="shared" si="3"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+      <c r="N45" s="50">
+        <v>36</v>
+      </c>
+      <c r="O45" s="51">
+        <f t="shared" si="4"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="P45" s="50">
+        <v>56</v>
+      </c>
+      <c r="Q45" s="51">
+        <f t="shared" si="5"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>17</v>
       </c>
@@ -1909,8 +3143,29 @@
       <c r="F46" s="15">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L46" s="25">
+        <v>17</v>
+      </c>
+      <c r="M46" s="36">
+        <f t="shared" si="3"/>
+        <v>1.3500000000000734E-3</v>
+      </c>
+      <c r="N46" s="25">
+        <v>37</v>
+      </c>
+      <c r="O46" s="36">
+        <f t="shared" si="4"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="P46" s="25">
+        <v>57</v>
+      </c>
+      <c r="Q46" s="36">
+        <f t="shared" si="5"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>18</v>
       </c>
@@ -1929,8 +3184,29 @@
       <c r="F47" s="15">
         <v>0.36899999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L47" s="50">
+        <v>18</v>
+      </c>
+      <c r="M47" s="51">
+        <f t="shared" si="3"/>
+        <v>3.3500000000000751E-3</v>
+      </c>
+      <c r="N47" s="50">
+        <v>38</v>
+      </c>
+      <c r="O47" s="51">
+        <f t="shared" si="4"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="P47" s="50">
+        <v>58</v>
+      </c>
+      <c r="Q47" s="51">
+        <f t="shared" si="5"/>
+        <v>-2.6499999999999302E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>19</v>
       </c>
@@ -1949,8 +3225,32 @@
       <c r="F48" s="15">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="25">
+        <v>19</v>
+      </c>
+      <c r="M48" s="36">
+        <f t="shared" si="3"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="N48" s="25">
+        <v>39</v>
+      </c>
+      <c r="O48" s="36">
+        <f t="shared" si="4"/>
+        <v>-6.4999999999992841E-4</v>
+      </c>
+      <c r="P48" s="25">
+        <v>59</v>
+      </c>
+      <c r="Q48" s="36">
+        <f t="shared" si="5"/>
+        <v>-1.6499999999999293E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>20</v>
       </c>
@@ -1969,19 +3269,68 @@
       <c r="F49" s="16">
         <v>0.372</v>
       </c>
+      <c r="H49" s="45">
+        <f>SUM(B30:B49,D30:D49,F30:F49)/60</f>
+        <v>0.37164999999999992</v>
+      </c>
+      <c r="L49" s="50">
+        <v>20</v>
+      </c>
+      <c r="M49" s="51">
+        <f t="shared" si="3"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+      <c r="N49" s="50">
+        <v>40</v>
+      </c>
+      <c r="O49" s="51">
+        <f t="shared" si="4"/>
+        <v>4.350000000000076E-3</v>
+      </c>
+      <c r="P49" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q49" s="51">
+        <f t="shared" si="5"/>
+        <v>3.5000000000007248E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L50" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="M50" s="31"/>
+      <c r="N50" s="32"/>
+      <c r="O50" s="42" cm="1">
+        <f t="array" ref="O50">SUM(ABS(M30:M49+O30:O49+Q30:Q49))/60</f>
+        <v>9.85000000000008E-4</v>
+      </c>
+      <c r="P50" s="43"/>
+      <c r="Q50" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="O50:Q50"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A26:F27"/>
     <mergeCell ref="H1:J2"/>
     <mergeCell ref="H8:J9"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="L27:Q27"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="S32:V32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AGORA SIMgit add *git add * FINALMENTE ACABOU
</commit_message>
<xml_diff>
--- a/EXP_2/Tabelas_EXP_2.xlsx
+++ b/EXP_2/Tabelas_EXP_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Filho\Documents\FISICA_1\EXP_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BB1F0B-8E07-4A9D-BA22-BD8E3D709E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BB200B-6ABC-4E41-88F2-9F669F41A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FCFF52A2-2253-4303-A898-002B8F5738EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FCFF52A2-2253-4303-A898-002B8F5738EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -494,38 +494,38 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1220,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC65827-CCCF-4375-835F-E03FB3F4C1AD}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25:Q25"/>
+    <sheetView tabSelected="1" topLeftCell="H24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50:Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,48 +1245,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="58" t="s">
+      <c r="L2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1529,11 +1529,11 @@
       <c r="F8" s="11">
         <v>0.48</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="3"/>
       <c r="L8" s="26">
         <v>4</v>
@@ -1576,9 +1576,9 @@
       <c r="F9" s="11">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
       <c r="K9" s="3"/>
       <c r="L9" s="25">
         <v>5</v>
@@ -2307,27 +2307,27 @@
         <v>5.3566666666666714E-2</v>
       </c>
       <c r="K25" s="3"/>
-      <c r="L25" s="52" t="s">
+      <c r="L25" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="M25" s="53"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="55" cm="1">
+      <c r="M25" s="56"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="58" cm="1">
         <f t="array" ref="O25">SUM(ABS(M5:M24+O5:O24+Q5:Q24))/60</f>
         <v>2.6783333333333357E-2</v>
       </c>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="57"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="60"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
       <c r="H26" s="38">
         <f>ABS(H24-H49)</f>
         <v>0.10451666666666692</v>
@@ -2336,30 +2336,30 @@
         <f>3*O25</f>
         <v>8.0350000000000074E-2</v>
       </c>
-      <c r="L26" s="58" t="s">
+      <c r="L26" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="L27" s="58" t="s">
+      <c r="A27" s="54"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="L27" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -2548,12 +2548,12 @@
         <f t="shared" si="5"/>
         <v>-2.6499999999999302E-3</v>
       </c>
-      <c r="S32" s="58" t="s">
+      <c r="S32" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="T32" s="58"/>
-      <c r="U32" s="58"/>
-      <c r="V32" s="58"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="54"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
@@ -2600,13 +2600,13 @@
         <v>24</v>
       </c>
       <c r="T33" s="44">
-        <v>0.48</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="U33" s="48" t="s">
         <v>27</v>
       </c>
       <c r="V33" s="49">
-        <v>5.3600000000000002E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="V34" s="51">
-        <v>8.0399999999999999E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -2706,13 +2706,12 @@
         <v>22</v>
       </c>
       <c r="T35" s="45">
-        <f>T33-T34</f>
-        <v>0.10799999999999998</v>
-      </c>
-      <c r="U35" s="61" t="s">
+        <v>0.104</v>
+      </c>
+      <c r="U35" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="V35" s="62"/>
+      <c r="V35" s="53"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
@@ -3296,17 +3295,17 @@
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L50" s="52" t="s">
+      <c r="L50" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="M50" s="53"/>
-      <c r="N50" s="54"/>
-      <c r="O50" s="55" cm="1">
+      <c r="M50" s="56"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="58" cm="1">
         <f t="array" ref="O50">SUM(ABS(M30:M49+O30:O49+Q30:Q49))/60</f>
         <v>9.85000000000008E-4</v>
       </c>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="57"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>